<commit_message>
replace space in group column names
</commit_message>
<xml_diff>
--- a/xls-to-xml-repeats.xlsx
+++ b/xls-to-xml-repeats.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3380" yWindow="1880" windowWidth="30100" windowHeight="9920"/>
+    <workbookView xWindow="0" yWindow="20" windowWidth="38460" windowHeight="9920" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Testing repeat forms" sheetId="1" r:id="rId1"/>
@@ -157,12 +157,6 @@
     <t>2017-11-29T21:06:32</t>
   </si>
   <si>
-    <t>Cooking Equipment</t>
-  </si>
-  <si>
-    <t>Years Owned</t>
-  </si>
-  <si>
     <t>_parent_table_name</t>
   </si>
   <si>
@@ -194,6 +188,12 @@
   </si>
   <si>
     <t>Food Processor</t>
+  </si>
+  <si>
+    <t>Cooking_Equipment</t>
+  </si>
+  <si>
+    <t>Years_Owned</t>
   </si>
 </sst>
 </file>
@@ -206,6 +206,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -564,7 +565,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
@@ -797,8 +798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -809,24 +810,24 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="B1" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="C1" t="s">
         <v>10</v>
       </c>
       <c r="D1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B2" t="s">
         <v>23</v>
@@ -835,7 +836,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -843,16 +844,16 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E3">
         <v>3</v>
@@ -860,16 +861,16 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E4">
         <v>3</v>
@@ -877,16 +878,16 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C5">
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E5">
         <v>4</v>
@@ -894,7 +895,7 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B6" t="s">
         <v>23</v>
@@ -903,7 +904,7 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E6">
         <v>4</v>
@@ -911,7 +912,7 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B7" t="s">
         <v>21</v>
@@ -920,7 +921,7 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E7">
         <v>5</v>

</xml_diff>